<commit_message>
Starting to model pricing and plans
</commit_message>
<xml_diff>
--- a/others/UML Diagram.xlsx
+++ b/others/UML Diagram.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\stock-management\others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A887D6FD-10C9-433A-8E44-70800958587D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE68118-06C1-4E02-B706-806BEEBC8780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1A83E2AC-DBC7-465A-80D2-ECE8A57E9D1A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1A83E2AC-DBC7-465A-80D2-ECE8A57E9D1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -193,7 +194,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="D38" authorId="15" shapeId="0" xr:uid="{3E87F653-930B-4A4F-BD04-B980DE216395}">
+    <comment ref="D39" authorId="15" shapeId="0" xr:uid="{3E87F653-930B-4A4F-BD04-B980DE216395}">
       <text>
         <t xml:space="preserve">[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -202,7 +203,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="F49" authorId="16" shapeId="0" xr:uid="{30F9FEC8-823C-43B6-BCD2-22C6F1961AEE}">
+    <comment ref="F50" authorId="16" shapeId="0" xr:uid="{30F9FEC8-823C-43B6-BCD2-22C6F1961AEE}">
       <text>
         <t xml:space="preserve">[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -216,7 +217,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="90">
   <si>
     <t>auth_assignment</t>
   </si>
@@ -417,6 +418,75 @@
   </si>
   <si>
     <t>linked_transaction_id</t>
+  </si>
+  <si>
+    <t>discount_rate</t>
+  </si>
+  <si>
+    <t>plan</t>
+  </si>
+  <si>
+    <t>plan_id</t>
+  </si>
+  <si>
+    <t>initial_date</t>
+  </si>
+  <si>
+    <t>final_date</t>
+  </si>
+  <si>
+    <t>Planes</t>
+  </si>
+  <si>
+    <t>Manejo de documentos</t>
+  </si>
+  <si>
+    <t>Manejo de productos</t>
+  </si>
+  <si>
+    <t>Manejo de bodegas</t>
+  </si>
+  <si>
+    <t>Manejo de proveedores</t>
+  </si>
+  <si>
+    <t>Realizacion de transacciones</t>
+  </si>
+  <si>
+    <t>Visualizacion de existencias y kardex</t>
+  </si>
+  <si>
+    <t>user_company_id</t>
+  </si>
+  <si>
+    <t>purchase</t>
+  </si>
+  <si>
+    <t>purchase_id</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>Gratis</t>
+  </si>
+  <si>
+    <t>Postular a empresas</t>
+  </si>
+  <si>
+    <t>Premium</t>
+  </si>
+  <si>
+    <t>Acceso a tu propia empresa</t>
+  </si>
+  <si>
+    <t>Manejo de personal</t>
+  </si>
+  <si>
+    <t>Si el owner ya tiene una licencia para una empresa comprada, hay un descuento para adquirir licencias para otra empresa.</t>
+  </si>
+  <si>
+    <t>Emprendedor</t>
   </si>
 </sst>
 </file>
@@ -572,7 +642,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -597,6 +667,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1566,6 +1639,106 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Conector recto 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A681DB60-8BE3-477E-EC94-FD6B697F0388}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1381125" y="4581525"/>
+          <a:ext cx="1295400" cy="581025"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Conector recto 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8B4BB6F-0290-4BED-BBBF-02CB9BB720D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1333500" y="7239000"/>
+          <a:ext cx="0" cy="581025"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1953,11 +2126,11 @@
     <text xml:space="preserve">Same as in user table
 </text>
   </threadedComment>
-  <threadedComment ref="D38" dT="2024-08-20T01:31:48.80" personId="{4707CDAA-3E59-4704-9530-1E3CAE3CC513}" id="{3E87F653-930B-4A4F-BD04-B980DE216395}">
+  <threadedComment ref="D39" dT="2024-08-20T01:31:48.80" personId="{4707CDAA-3E59-4704-9530-1E3CAE3CC513}" id="{3E87F653-930B-4A4F-BD04-B980DE216395}">
     <text xml:space="preserve">Same as in user table
 </text>
   </threadedComment>
-  <threadedComment ref="F49" dT="2024-08-20T01:32:03.36" personId="{4707CDAA-3E59-4704-9530-1E3CAE3CC513}" id="{30F9FEC8-823C-43B6-BCD2-22C6F1961AEE}">
+  <threadedComment ref="F50" dT="2024-08-20T01:32:03.36" personId="{4707CDAA-3E59-4704-9530-1E3CAE3CC513}" id="{30F9FEC8-823C-43B6-BCD2-22C6F1961AEE}">
     <text xml:space="preserve">Same as in user table
 </text>
   </threadedComment>
@@ -1966,15 +2139,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA726A6-B4C5-4E14-AD97-EDC1C42AA14F}">
-  <dimension ref="B2:L53"/>
+  <dimension ref="B2:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -2342,6 +2515,9 @@
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="D28" s="5" t="s">
         <v>40</v>
       </c>
@@ -2356,6 +2532,9 @@
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="23" t="s">
+        <v>81</v>
+      </c>
       <c r="D29" s="13" t="s">
         <v>41</v>
       </c>
@@ -2370,6 +2549,9 @@
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="24" t="s">
+        <v>79</v>
+      </c>
       <c r="D30" s="14" t="s">
         <v>29</v>
       </c>
@@ -2384,6 +2566,9 @@
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="24" t="s">
+        <v>69</v>
+      </c>
       <c r="D31" s="14" t="s">
         <v>5</v>
       </c>
@@ -2398,6 +2583,9 @@
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="22" t="s">
+        <v>70</v>
+      </c>
       <c r="D32" s="14" t="s">
         <v>7</v>
       </c>
@@ -2411,7 +2599,10 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="22" t="s">
+        <v>71</v>
+      </c>
       <c r="D33" s="15" t="s">
         <v>28</v>
       </c>
@@ -2425,7 +2616,10 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="22" t="s">
+        <v>24</v>
+      </c>
       <c r="D34" s="21" t="s">
         <v>64</v>
       </c>
@@ -2439,7 +2633,10 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="22" t="s">
+        <v>25</v>
+      </c>
       <c r="D35" s="14" t="s">
         <v>49</v>
       </c>
@@ -2453,9 +2650,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D36" s="14" t="s">
-        <v>42</v>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>67</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>3</v>
@@ -2467,9 +2667,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="22" t="s">
+        <v>3</v>
+      </c>
       <c r="D37" s="14" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>10</v>
@@ -2481,25 +2684,28 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="22" t="s">
+        <v>10</v>
+      </c>
       <c r="D38" s="14" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="J38" s="19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D39" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J39" s="19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D40" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>46</v>
@@ -2508,9 +2714,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D41" s="14" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="F41" s="17" t="s">
         <v>47</v>
@@ -2519,72 +2725,214 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="D42" s="14" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F42" s="18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>10</v>
+      </c>
       <c r="F43" s="19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="22" t="s">
+        <v>5</v>
+      </c>
       <c r="F44" s="19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="22" t="s">
+        <v>7</v>
+      </c>
       <c r="F45" s="19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="F46" s="18" t="s">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="F46" s="20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B47" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="F47" s="18" t="s">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="F48" s="18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="F48" s="18" t="s">
+    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F49" s="18" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F49" s="19" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="50" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F50" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F51" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F52" s="19" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
     </row>
     <row r="53" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F53" s="19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F54" s="19" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1201CE7C-8DA8-42A7-B0C5-597DD7DD29BC}">
+  <dimension ref="B3:C19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>